<commit_message>
Visualization in R pretty much finished Nedd to integrate with rest of pipleine
</commit_message>
<xml_diff>
--- a/Data/Improving Script.xlsx
+++ b/Data/Improving Script.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasco\OneDrive\Documents\Bioinformatics\Immunodietica\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{332C2BE3-4B79-4A26-856C-14A878104B4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{29C9EE21-9508-43F3-8AE9-80A73CFB4071}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="8_{332C2BE3-4B79-4A26-856C-14A878104B4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{25B9C9FA-FF98-4A82-AB8D-5682D372158F}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{7318A47C-9809-441E-8437-84BDBEF0C691}"/>
+    <workbookView xWindow="4410" yWindow="1965" windowWidth="13260" windowHeight="11423" activeTab="1" xr2:uid="{7318A47C-9809-441E-8437-84BDBEF0C691}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>Pig MS Epitopes</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Full Epitope Set</t>
+  </si>
+  <si>
+    <t>Full Epitope Set (18829)</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1115,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E6AA1DB-43B6-42C2-94C1-5E4DEB6BAC96}" type="CELLRANGE">
+                    <a:fld id="{069CCF48-2269-4704-BF2E-93FAA3F605EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1145,7 +1148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{802C1514-34BF-4B01-860A-463D29E390C6}" type="CELLRANGE">
+                    <a:fld id="{55B954F7-45FE-47DE-AEB6-E15CAAD22D7C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1178,7 +1181,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2791B4E8-DE99-41B6-A8CF-B6FFED1CFECF}" type="CELLRANGE">
+                    <a:fld id="{D0473359-BFF3-4955-8161-D5907BA6C7D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1211,7 +1214,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3BAE0672-776C-40D9-9C5D-5F2605CA5277}" type="CELLRANGE">
+                    <a:fld id="{69729898-D2BC-4D72-900B-58C86EA0F570}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1244,7 +1247,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A572307-0B9C-49D7-A99D-A57072DC6839}" type="CELLRANGE">
+                    <a:fld id="{256DC89C-7C72-40A5-9B62-A7472DCBCBA3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1277,7 +1280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3AA2FF35-75FB-4D0F-8ED0-CC77C788FEB9}" type="CELLRANGE">
+                    <a:fld id="{86515DF2-4AD8-4DEF-9B16-39D4A8FC9FBD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1485,7 +1488,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{905E5E40-0BA7-40CB-93B4-30474FF1325D}" type="CELLRANGE">
+                    <a:fld id="{9840F9AE-968F-4FBF-93DE-57234E05B9E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1518,7 +1521,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CBA0D2C-2301-45FA-85BB-F20304D7BD62}" type="CELLRANGE">
+                    <a:fld id="{48B00E36-5A69-4FA0-9721-983253805B78}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1551,7 +1554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96C34F45-6F3B-47E8-9D7A-52F6A2D76F8C}" type="CELLRANGE">
+                    <a:fld id="{C451D56B-66A9-47A6-8DC4-260076C3B79E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1584,7 +1587,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{55ED9DAF-20D3-4A87-8B0C-4FC3DFB7DB2B}" type="CELLRANGE">
+                    <a:fld id="{B6EA91CA-740C-47F5-B8EC-92F83BEBD011}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1617,7 +1620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5825D347-6432-46FF-BD26-242F1E583FDD}" type="CELLRANGE">
+                    <a:fld id="{60D7662A-DC65-41FF-8696-3FC069D0FDC0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1650,7 +1653,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A0DEB3B8-9547-4CF4-A49D-E5867BC2DD41}" type="CELLRANGE">
+                    <a:fld id="{0E56046B-7DAB-447E-9137-30F835DA394D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1858,7 +1861,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2C72C33-1127-4EBC-8B10-62663919114B}" type="CELLRANGE">
+                    <a:fld id="{A410C146-7983-48A5-A578-01A1CC74BE0A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1891,7 +1894,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E6A92A1-89BE-4AB7-99DE-624CACBC4C9C}" type="CELLRANGE">
+                    <a:fld id="{A652B96F-C31C-4D4D-B3A4-3F9FA2AD6C6F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1924,7 +1927,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A98F133D-C43E-4B9E-B069-0ECCA3EE0559}" type="CELLRANGE">
+                    <a:fld id="{D40215D2-72E4-4A57-849E-E98579261574}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1957,7 +1960,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF125D0A-6F44-4261-B5B9-26CA2328243D}" type="CELLRANGE">
+                    <a:fld id="{88E66063-7C07-4729-8F28-2112A942463E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1990,7 +1993,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B86797FC-0079-44AD-952A-725B9A6A1B97}" type="CELLRANGE">
+                    <a:fld id="{548A957D-5CAE-4054-A711-9FC8260B6872}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2023,7 +2026,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3FC76B54-96C3-4319-897D-40F0601A0002}" type="CELLRANGE">
+                    <a:fld id="{8D571374-16C8-4324-B5E2-50CBC3D6D997}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2196,6 +2199,904 @@
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-91A3-4660-951A-D0D50471C739}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="504594911"/>
+        <c:axId val="570789503"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="504594911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="570789503"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="570789503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="504594911"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2800"/>
+              <a:t>Full Epitope Set</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2800" baseline="0"/>
+              <a:t> (18,829)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19545182495080043"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UniProt (SwissProt Query)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0CB40FEF-2833-487D-A828-A93425170098}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-E066-4142-8F75-48E8D89DBE39}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E2CEB891-55B3-4188-81B5-BE2D38A5B082}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-E066-4142-8F75-48E8D89DBE39}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$H$9:$I$10</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>ACC ID</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Protein Name</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Full Epitope Set (18829)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>80.869934675235015</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88.193743693239156</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Sheet1!$H$4:$I$4</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>15227</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>16606</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-E066-4142-8F75-48E8D89DBE39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gene Symbol (db2db Query)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{ED6ED1AC-E077-4627-888A-D5F4F8CCC473}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-E066-4142-8F75-48E8D89DBE39}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{54C18AD2-84EF-4BDC-9EE7-82365B355685}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-E066-4142-8F75-48E8D89DBE39}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$H$9:$I$10</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>ACC ID</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Protein Name</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Full Epitope Set (18829)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$12:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>75.07037017366828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.765946146901058</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Sheet1!$H$6:$I$6</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>14135</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>15584</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-E066-4142-8F75-48E8D89DBE39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unmatched (SwissProt Query)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{564AF60D-19D0-4891-8DBB-4C66C373069E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-E066-4142-8F75-48E8D89DBE39}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{48A475CF-EC9D-4787-A5AC-58FF1F09C946}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-E066-4142-8F75-48E8D89DBE39}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$H$9:$I$10</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>ACC ID</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Protein Name</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Full Epitope Set (18829)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$13:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>19.406235062934833</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.593818046630199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Sheet1!$H$5:$I$5</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>3654</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2183</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000014-E066-4142-8F75-48E8D89DBE39}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2482,6 +3383,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -2988,6 +3929,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3567,6 +5011,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133306</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>632033</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>80709</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{098463A5-5468-4E3F-930D-7FAEB7A7C942}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3874,8 +5356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEAF529A-DBED-4B16-B91D-0394F00F2EFD}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="E23" zoomScale="107" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4045,7 +5527,7 @@
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9">

</xml_diff>